<commit_message>
fine tuning graph labels, sizes
</commit_message>
<xml_diff>
--- a/water_quality/data_raw/Water quality data.xlsx
+++ b/water_quality/data_raw/Water quality data.xlsx
@@ -130,7 +130,7 @@
     <t>DB</t>
   </si>
   <si>
-    <t>Exchange Bay - Dansby</t>
+    <t>Exchange Bay - Turtle Beach</t>
   </si>
   <si>
     <t>MRCH</t>
@@ -178,7 +178,7 @@
     <t>BDB</t>
   </si>
   <si>
-    <t>Big Deep Bay</t>
+    <t>Great Deep Bay</t>
   </si>
   <si>
     <t>LDB</t>

</xml_diff>